<commit_message>
missing break added with time
</commit_message>
<xml_diff>
--- a/Sprungdaten Innotramp/2019.09.30/Sprungzuordnung_Nachmittag-20190930-1616-FRANKFURT_1-01.XLSX
+++ b/Sprungdaten Innotramp/2019.09.30/Sprungzuordnung_Nachmittag-20190930-1616-FRANKFURT_1-01.XLSX
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tabellen Sprungerkennung\2019.09.30\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Komplexpraktikum\Trampolin\Sprungdaten Innotramp\2019.09.30\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90028DA5-98B8-4AC3-86CE-518B964D43AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26940" windowHeight="13785"/>
+    <workbookView xWindow="29340" yWindow="855" windowWidth="18720" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phasentabelle.mms" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="215">
   <si>
     <t>Event</t>
   </si>
@@ -666,12 +667,15 @@
   </si>
   <si>
     <t>1 3/4 salto Vorwärts B</t>
+  </si>
+  <si>
+    <t>317.480 sec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -719,7 +723,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -736,6 +740,7 @@
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1015,11 +1020,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N367"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A337" workbookViewId="0">
-      <selection activeCell="F365" sqref="F365"/>
+    <sheetView tabSelected="1" topLeftCell="A322" workbookViewId="0">
+      <selection activeCell="G363" sqref="G363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16533,8 +16538,8 @@
       <c r="E354">
         <v>0</v>
       </c>
-      <c r="F354" t="s">
-        <v>201</v>
+      <c r="G354" s="8" t="s">
+        <v>214</v>
       </c>
       <c r="H354">
         <v>0</v>

</xml_diff>